<commit_message>
Updated code add V2
</commit_message>
<xml_diff>
--- a/Input_Data/RunnerData.xlsx
+++ b/Input_Data/RunnerData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PythonProjects\PDFValidator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PythonProjects\PDFValidator\Input_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA71058-9413-4893-8BF5-72D3668E6111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6773E1-66B1-4586-B218-7797E0C22F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>Img</t>
   </si>
   <si>
-    <t>C:\Users\MR.ROBOT\Desktop\Untitled.png</t>
-  </si>
-  <si>
     <t>D:\Projects\PythonProjects\PDFValidator\PDF</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>top right</t>
+  </si>
+  <si>
+    <t>C:\Users\username\Desktop\Untitled.png</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,10 +443,10 @@
     </row>
     <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -458,15 +458,15 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -478,15 +478,15 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -498,15 +498,15 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -515,18 +515,18 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -535,18 +535,18 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>

</xml_diff>